<commit_message>
insert rtt load in one hop
</commit_message>
<xml_diff>
--- a/ModelingV0/output/data/teste.xlsx
+++ b/ModelingV0/output/data/teste.xlsx
@@ -488,22 +488,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['00000001_F9']</t>
+          <t>['00000001_F3']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['F9']</t>
+          <t>['F3']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['UE17']</t>
+          <t>['UE48']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['F9', 'SBS2', 'UE17']</t>
+          <t>['F3', 'SBS2', 'UE48']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -521,22 +521,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['00000001_F9']</t>
+          <t>['00000001_F3']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['F9']</t>
+          <t>['F3']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['UE17']</t>
+          <t>['UE48']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['F9', 'SBS2', 'UE17']</t>
+          <t>['F3', 'SBS2', 'UE48']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -554,27 +554,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['00000002_F6']</t>
+          <t>['00000002_F9']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['F6']</t>
+          <t>['F9']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['UE31']</t>
+          <t>['UE29']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['F6', 'SBS2', 'UE31']</t>
+          <t>['F9', 'SBS4', 'UE29']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>SBS2</t>
+          <t>SBS4</t>
         </is>
       </c>
     </row>
@@ -587,22 +587,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['00000001_F9']</t>
+          <t>['00000001_F3']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['F9']</t>
+          <t>['F3']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['UE17']</t>
+          <t>['UE48']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['F9', 'SBS2', 'UE17']</t>
+          <t>['F3', 'SBS2', 'UE48']</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -620,27 +620,27 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['00000002_F6']</t>
+          <t>['00000002_F9']</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['F6']</t>
+          <t>['F9']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['UE31']</t>
+          <t>['UE29']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['F6', 'SBS3', 'UE31']</t>
+          <t>['F9', 'SBS4', 'UE29']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>SBS3</t>
+          <t>SBS4</t>
         </is>
       </c>
     </row>
@@ -653,27 +653,27 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['00000003_F2']</t>
+          <t>['00000003_F1']</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['F2']</t>
+          <t>['F1']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['UE49']</t>
+          <t>['UE43']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>['F2', 'SBS2', 'UE49']</t>
+          <t>['F1', 'SBS3', 'UE43']</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>SBS2</t>
+          <t>SBS3</t>
         </is>
       </c>
     </row>
@@ -686,22 +686,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['00000001_F9']</t>
+          <t>['00000001_F3']</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['F9']</t>
+          <t>['F3']</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['UE17']</t>
+          <t>['UE48']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['F9', 'SBS2', 'UE17']</t>
+          <t>['F3', 'SBS2', 'UE48']</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -719,27 +719,27 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['00000002_F6']</t>
+          <t>['00000002_F9']</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['F6']</t>
+          <t>['F9']</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>['UE31']</t>
+          <t>['UE29']</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['F6', 'SBS2', 'UE31']</t>
+          <t>['F9', 'SBS1', 'UE29']</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>SBS2</t>
+          <t>SBS1</t>
         </is>
       </c>
     </row>
@@ -752,27 +752,27 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['00000003_F2']</t>
+          <t>['00000003_F1']</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['F2']</t>
+          <t>['F1']</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['UE49']</t>
+          <t>['UE43']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['F2', 'MBS0', 'UE49']</t>
+          <t>['F1', 'SBS3', 'UE43']</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>MBS0</t>
+          <t>SBS3</t>
         </is>
       </c>
     </row>
@@ -785,27 +785,27 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['00000004_F2']</t>
+          <t>['00000004_F1']</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['F2']</t>
+          <t>['F1']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['UE42']</t>
+          <t>['UE32']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['F2', 'MBS0', 'UE42']</t>
+          <t>['F1', 'SBS3', 'UE32']</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>MBS0</t>
+          <t>SBS3</t>
         </is>
       </c>
     </row>
@@ -818,27 +818,27 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['00000001_F9']</t>
+          <t>['00000001_F3']</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['F9']</t>
+          <t>['F3']</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['UE17']</t>
+          <t>['UE48']</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['F9', 'SBS2', 'UE17']</t>
+          <t>['F3', 'MBS0', 'UE48']</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>SBS2</t>
+          <t>MBS0</t>
         </is>
       </c>
     </row>
@@ -851,27 +851,27 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['00000002_F6']</t>
+          <t>['00000002_F9']</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['F6']</t>
+          <t>['F9']</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['UE31']</t>
+          <t>['UE29']</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['F6', 'SBS2', 'UE31']</t>
+          <t>['F9', 'SBS1', 'UE29']</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>SBS2</t>
+          <t>SBS1</t>
         </is>
       </c>
     </row>
@@ -884,27 +884,27 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['00000003_F2']</t>
+          <t>['00000003_F1']</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>['F2']</t>
+          <t>['F1']</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['UE49']</t>
+          <t>['UE43']</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['F2', 'MBS0', 'UE49']</t>
+          <t>['F1', 'SBS3', 'UE43']</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>MBS0</t>
+          <t>SBS3</t>
         </is>
       </c>
     </row>
@@ -917,27 +917,27 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['00000004_F2']</t>
+          <t>['00000004_F1']</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>['F2']</t>
+          <t>['F1']</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>['UE42']</t>
+          <t>['UE32']</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>['F2', 'MBS0', 'UE42']</t>
+          <t>['F1', 'SBS3', 'UE32']</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>MBS0</t>
+          <t>SBS3</t>
         </is>
       </c>
     </row>
@@ -950,22 +950,22 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['00000005_F2']</t>
+          <t>['00000005_F3']</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>['F2']</t>
+          <t>['F3']</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>['UE2']</t>
+          <t>['UE25']</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['F2', 'MBS0', 'UE2']</t>
+          <t>['F3', 'MBS0', 'UE25']</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -983,27 +983,27 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['00000001_F9']</t>
+          <t>['00000001_F3']</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>['F9']</t>
+          <t>['F3']</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>['UE17']</t>
+          <t>['UE48']</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>['F9', 'SBS2', 'UE17']</t>
+          <t>['F3', 'MBS0', 'UE48']</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>SBS2</t>
+          <t>MBS0</t>
         </is>
       </c>
     </row>
@@ -1016,27 +1016,27 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>['00000002_F6']</t>
+          <t>['00000002_F9']</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>['F6']</t>
+          <t>['F9']</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>['UE31']</t>
+          <t>['UE29']</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>['F6', 'MBS0', 'UE31']</t>
+          <t>['F9', 'SBS1', 'UE29']</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>MBS0</t>
+          <t>SBS1</t>
         </is>
       </c>
     </row>
@@ -1049,27 +1049,27 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['00000003_F2']</t>
+          <t>['00000003_F1']</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['F2']</t>
+          <t>['F1']</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>['UE49']</t>
+          <t>['UE43']</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>['F2', 'MBS0', 'UE49']</t>
+          <t>['F1', 'SBS3', 'UE43']</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>MBS0</t>
+          <t>SBS3</t>
         </is>
       </c>
     </row>
@@ -1082,27 +1082,27 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>['00000004_F2']</t>
+          <t>['00000004_F1']</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>['F2']</t>
+          <t>['F1']</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>['UE42']</t>
+          <t>['UE32']</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>['F2', 'MBS0', 'UE42']</t>
+          <t>['F1', 'SBS3', 'UE32']</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>MBS0</t>
+          <t>SBS3</t>
         </is>
       </c>
     </row>
@@ -1115,22 +1115,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>['00000005_F2']</t>
+          <t>['00000005_F3']</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['F2']</t>
+          <t>['F3']</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>['UE2']</t>
+          <t>['UE25']</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>['F2', 'MBS0', 'UE2']</t>
+          <t>['F3', 'MBS0', 'UE25']</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1148,27 +1148,27 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>['00000006_F6']</t>
+          <t>['00000006_F5']</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>['F6']</t>
+          <t>['F5']</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>['UE24']</t>
+          <t>['UE2']</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>['F6', 'MBS0', 'UE24']</t>
+          <t>['F5', 'SBS2', 'UE2']</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>MBS0</t>
+          <t>SBS2</t>
         </is>
       </c>
     </row>
@@ -1232,7 +1232,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1259,11 +1259,7 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>00000002_F6</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1274,7 +1270,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>00000002_F6</t>
+          <t>00000002_F9</t>
         </is>
       </c>
     </row>
@@ -1287,20 +1283,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>00000003_F2</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>00000002_F6</t>
+          <t>00000001_F3</t>
         </is>
       </c>
     </row>
@@ -1378,7 +1361,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>F9</t>
+          <t>F3</t>
         </is>
       </c>
     </row>
@@ -1388,7 +1371,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>F6</t>
+          <t>F9</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1381,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>F2</t>
+          <t>F1</t>
         </is>
       </c>
     </row>
@@ -1408,7 +1391,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>F2</t>
+          <t>F1</t>
         </is>
       </c>
     </row>
@@ -1418,7 +1401,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>F2</t>
+          <t>F3</t>
         </is>
       </c>
     </row>
@@ -1428,7 +1411,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>F6</t>
+          <t>F5</t>
         </is>
       </c>
     </row>
@@ -1443,7 +1426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E261"/>
+  <dimension ref="A1:E262"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3956,10 +3939,10 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E132" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="133">
@@ -3975,10 +3958,10 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E133" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="134">
@@ -3994,10 +3977,10 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E134" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="135">
@@ -4013,10 +3996,10 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E135" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="136">
@@ -4032,10 +4015,10 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E136" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="137">
@@ -4051,10 +4034,10 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E137" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="138">
@@ -4070,10 +4053,10 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E138" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="139">
@@ -4089,10 +4072,10 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E139" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="140">
@@ -4108,10 +4091,10 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E140" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="141">
@@ -4127,10 +4110,10 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E141" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="142">
@@ -4146,10 +4129,10 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E142" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="143">
@@ -4165,10 +4148,10 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E143" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="144">
@@ -4184,10 +4167,10 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E144" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="145">
@@ -4203,10 +4186,10 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E145" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="146">
@@ -4222,10 +4205,10 @@
         </is>
       </c>
       <c r="D146" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E146" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="147">
@@ -4241,10 +4224,10 @@
         </is>
       </c>
       <c r="D147" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E147" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="148">
@@ -4260,10 +4243,10 @@
         </is>
       </c>
       <c r="D148" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E148" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="149">
@@ -4279,10 +4262,10 @@
         </is>
       </c>
       <c r="D149" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E149" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="150">
@@ -4298,10 +4281,10 @@
         </is>
       </c>
       <c r="D150" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E150" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="151">
@@ -4317,10 +4300,10 @@
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E151" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="152">
@@ -4336,10 +4319,10 @@
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E152" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="153">
@@ -4355,10 +4338,10 @@
         </is>
       </c>
       <c r="D153" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E153" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="154">
@@ -4374,10 +4357,10 @@
         </is>
       </c>
       <c r="D154" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E154" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="155">
@@ -4393,10 +4376,10 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E155" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="156">
@@ -4412,10 +4395,10 @@
         </is>
       </c>
       <c r="D156" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E156" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="157">
@@ -4431,10 +4414,10 @@
         </is>
       </c>
       <c r="D157" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E157" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="158">
@@ -4450,10 +4433,10 @@
         </is>
       </c>
       <c r="D158" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E158" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="159">
@@ -4469,10 +4452,10 @@
         </is>
       </c>
       <c r="D159" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E159" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="160">
@@ -4488,10 +4471,10 @@
         </is>
       </c>
       <c r="D160" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E160" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="161">
@@ -4507,10 +4490,10 @@
         </is>
       </c>
       <c r="D161" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E161" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="162">
@@ -4526,10 +4509,10 @@
         </is>
       </c>
       <c r="D162" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E162" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="163">
@@ -4545,10 +4528,10 @@
         </is>
       </c>
       <c r="D163" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E163" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="164">
@@ -4564,10 +4547,10 @@
         </is>
       </c>
       <c r="D164" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E164" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="165">
@@ -4583,10 +4566,10 @@
         </is>
       </c>
       <c r="D165" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E165" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="166">
@@ -4602,10 +4585,10 @@
         </is>
       </c>
       <c r="D166" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E166" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="167">
@@ -4621,10 +4604,10 @@
         </is>
       </c>
       <c r="D167" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E167" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="168">
@@ -4640,10 +4623,10 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E168" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="169">
@@ -4659,10 +4642,10 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E169" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="170">
@@ -4678,10 +4661,10 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E170" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="171">
@@ -4697,10 +4680,10 @@
         </is>
       </c>
       <c r="D171" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E171" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="172">
@@ -4716,10 +4699,10 @@
         </is>
       </c>
       <c r="D172" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E172" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="173">
@@ -4735,10 +4718,10 @@
         </is>
       </c>
       <c r="D173" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E173" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="174">
@@ -4754,10 +4737,10 @@
         </is>
       </c>
       <c r="D174" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E174" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="175">
@@ -4773,10 +4756,10 @@
         </is>
       </c>
       <c r="D175" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E175" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="176">
@@ -4792,10 +4775,10 @@
         </is>
       </c>
       <c r="D176" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E176" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="177">
@@ -4811,10 +4794,10 @@
         </is>
       </c>
       <c r="D177" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E177" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="178">
@@ -4830,10 +4813,10 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E178" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="179">
@@ -4849,10 +4832,10 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E179" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="180">
@@ -4868,10 +4851,10 @@
         </is>
       </c>
       <c r="D180" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E180" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="181">
@@ -4887,10 +4870,10 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E181" t="n">
-        <v>12000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="182">
@@ -5058,10 +5041,10 @@
         </is>
       </c>
       <c r="D190" t="n">
-        <v>0.001386</v>
+        <v>0.0011</v>
       </c>
       <c r="E190" t="n">
-        <v>34632</v>
+        <v>43636</v>
       </c>
     </row>
     <row r="191">
@@ -5077,10 +5060,10 @@
         </is>
       </c>
       <c r="D191" t="n">
-        <v>0.001143</v>
+        <v>0.001429</v>
       </c>
       <c r="E191" t="n">
-        <v>41995</v>
+        <v>33590</v>
       </c>
     </row>
     <row r="192">
@@ -5096,10 +5079,10 @@
         </is>
       </c>
       <c r="D192" t="n">
-        <v>0.001</v>
+        <v>0.001243</v>
       </c>
       <c r="E192" t="n">
-        <v>48000</v>
+        <v>38616</v>
       </c>
     </row>
     <row r="193">
@@ -5115,10 +5098,10 @@
         </is>
       </c>
       <c r="D193" t="n">
-        <v>0.0012</v>
+        <v>0.001486</v>
       </c>
       <c r="E193" t="n">
-        <v>40000</v>
+        <v>32301</v>
       </c>
     </row>
     <row r="194">
@@ -5153,10 +5136,10 @@
         </is>
       </c>
       <c r="D195" t="n">
-        <v>0.001614</v>
+        <v>0.001329</v>
       </c>
       <c r="E195" t="n">
-        <v>29740</v>
+        <v>36117</v>
       </c>
     </row>
     <row r="196">
@@ -5172,10 +5155,10 @@
         </is>
       </c>
       <c r="D196" t="n">
-        <v>0.001171</v>
+        <v>0.001</v>
       </c>
       <c r="E196" t="n">
-        <v>40991</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="197">
@@ -5248,10 +5231,10 @@
         </is>
       </c>
       <c r="D200" t="n">
-        <v>0.001686</v>
+        <v>0.001971</v>
       </c>
       <c r="E200" t="n">
-        <v>28470</v>
+        <v>24353</v>
       </c>
     </row>
     <row r="201">
@@ -5267,10 +5250,10 @@
         </is>
       </c>
       <c r="D201" t="n">
-        <v>0.0012</v>
+        <v>0.001</v>
       </c>
       <c r="E201" t="n">
-        <v>40000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="202">
@@ -5286,10 +5269,10 @@
         </is>
       </c>
       <c r="D202" t="n">
-        <v>0.001171</v>
+        <v>0.001457</v>
       </c>
       <c r="E202" t="n">
-        <v>40991</v>
+        <v>32944</v>
       </c>
     </row>
     <row r="203">
@@ -5305,10 +5288,10 @@
         </is>
       </c>
       <c r="D203" t="n">
-        <v>0.001457</v>
+        <v>0.001743</v>
       </c>
       <c r="E203" t="n">
-        <v>32944</v>
+        <v>27539</v>
       </c>
     </row>
     <row r="204">
@@ -5339,14 +5322,14 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE47')</t>
+          <t>('SBS1', 'UE48')</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>0.001929</v>
+        <v>0.001729</v>
       </c>
       <c r="E205" t="n">
-        <v>24883</v>
+        <v>27762</v>
       </c>
     </row>
     <row r="206">
@@ -5358,14 +5341,14 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE48')</t>
+          <t>('SBS2', 'MBS1')</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>0.001729</v>
+        <v>0.002</v>
       </c>
       <c r="E206" t="n">
-        <v>27762</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="207">
@@ -5377,14 +5360,14 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>('SBS2', 'MBS1')</t>
+          <t>('SBS2', 'UE2')</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>0.002</v>
+        <v>0.0014</v>
       </c>
       <c r="E207" t="n">
-        <v>24000</v>
+        <v>34286</v>
       </c>
     </row>
     <row r="208">
@@ -5396,14 +5379,14 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE2')</t>
+          <t>('SBS2', 'UE4')</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>0.001114</v>
+        <v>0.001457</v>
       </c>
       <c r="E208" t="n">
-        <v>43088</v>
+        <v>32944</v>
       </c>
     </row>
     <row r="209">
@@ -5415,14 +5398,14 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE4')</t>
+          <t>('SBS2', 'UE10')</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>0.001457</v>
+        <v>0.001929</v>
       </c>
       <c r="E209" t="n">
-        <v>32944</v>
+        <v>24883</v>
       </c>
     </row>
     <row r="210">
@@ -5434,14 +5417,14 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE10')</t>
+          <t>('SBS2', 'UE14')</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>0.001643</v>
+        <v>0.001843</v>
       </c>
       <c r="E210" t="n">
-        <v>29215</v>
+        <v>26044</v>
       </c>
     </row>
     <row r="211">
@@ -5453,14 +5436,14 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE14')</t>
+          <t>('SBS2', 'UE17')</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>0.001843</v>
+        <v>0.001943</v>
       </c>
       <c r="E211" t="n">
-        <v>26044</v>
+        <v>24704</v>
       </c>
     </row>
     <row r="212">
@@ -5472,14 +5455,14 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE17')</t>
+          <t>('SBS2', 'UE19')</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>0.001943</v>
+        <v>0.001986</v>
       </c>
       <c r="E212" t="n">
-        <v>24704</v>
+        <v>24169</v>
       </c>
     </row>
     <row r="213">
@@ -5491,14 +5474,14 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE19')</t>
+          <t>('SBS2', 'UE20')</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>0.001986</v>
+        <v>0.001786</v>
       </c>
       <c r="E213" t="n">
-        <v>24169</v>
+        <v>26876</v>
       </c>
     </row>
     <row r="214">
@@ -5510,14 +5493,14 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE20')</t>
+          <t>('SBS2', 'UE21')</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>0.0019</v>
+        <v>0.001529</v>
       </c>
       <c r="E214" t="n">
-        <v>25263</v>
+        <v>31393</v>
       </c>
     </row>
     <row r="215">
@@ -5529,14 +5512,14 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE21')</t>
+          <t>('SBS2', 'UE22')</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>0.001529</v>
+        <v>0.001986</v>
       </c>
       <c r="E215" t="n">
-        <v>31393</v>
+        <v>24169</v>
       </c>
     </row>
     <row r="216">
@@ -5548,14 +5531,14 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE22')</t>
+          <t>('SBS2', 'UE30')</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>0.001986</v>
+        <v>0.001943</v>
       </c>
       <c r="E216" t="n">
-        <v>24169</v>
+        <v>24704</v>
       </c>
     </row>
     <row r="217">
@@ -5567,14 +5550,14 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE30')</t>
+          <t>('SBS2', 'UE31')</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>0.001943</v>
+        <v>0.001</v>
       </c>
       <c r="E217" t="n">
-        <v>24704</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="218">
@@ -5586,14 +5569,14 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE31')</t>
+          <t>('SBS2', 'UE41')</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>0.001</v>
+        <v>0.0016</v>
       </c>
       <c r="E218" t="n">
-        <v>48000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="219">
@@ -5605,14 +5588,14 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE41')</t>
+          <t>('SBS2', 'UE48')</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>0.0016</v>
+        <v>0.001443</v>
       </c>
       <c r="E219" t="n">
-        <v>30000</v>
+        <v>33264</v>
       </c>
     </row>
     <row r="220">
@@ -5624,14 +5607,14 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE48')</t>
+          <t>('SBS2', 'UE49')</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>0.001443</v>
+        <v>0.001314</v>
       </c>
       <c r="E220" t="n">
-        <v>33264</v>
+        <v>36530</v>
       </c>
     </row>
     <row r="221">
@@ -5643,14 +5626,14 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE49')</t>
+          <t>('SBS2', 'UE50')</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>0.001314</v>
+        <v>0.0018</v>
       </c>
       <c r="E221" t="n">
-        <v>36530</v>
+        <v>26667</v>
       </c>
     </row>
     <row r="222">
@@ -5662,14 +5645,14 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE50')</t>
+          <t>('SBS3', 'MBS2')</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>0.0018</v>
+        <v>0.002</v>
       </c>
       <c r="E222" t="n">
-        <v>26667</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="223">
@@ -5681,14 +5664,14 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>('SBS3', 'MBS2')</t>
+          <t>('SBS3', 'UE1')</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>0.002</v>
+        <v>0.001957</v>
       </c>
       <c r="E223" t="n">
-        <v>24000</v>
+        <v>24527</v>
       </c>
     </row>
     <row r="224">
@@ -5723,10 +5706,10 @@
         </is>
       </c>
       <c r="D225" t="n">
-        <v>0.001086</v>
+        <v>0.001371</v>
       </c>
       <c r="E225" t="n">
-        <v>44199</v>
+        <v>35011</v>
       </c>
     </row>
     <row r="226">
@@ -5761,10 +5744,10 @@
         </is>
       </c>
       <c r="D227" t="n">
-        <v>0.001571</v>
+        <v>0.001286</v>
       </c>
       <c r="E227" t="n">
-        <v>30554</v>
+        <v>37325</v>
       </c>
     </row>
     <row r="228">
@@ -5780,10 +5763,10 @@
         </is>
       </c>
       <c r="D228" t="n">
-        <v>0.001286</v>
+        <v>0.001571</v>
       </c>
       <c r="E228" t="n">
-        <v>37325</v>
+        <v>30554</v>
       </c>
     </row>
     <row r="229">
@@ -5799,10 +5782,10 @@
         </is>
       </c>
       <c r="D229" t="n">
-        <v>0.001443</v>
+        <v>0.001157</v>
       </c>
       <c r="E229" t="n">
-        <v>33264</v>
+        <v>41487</v>
       </c>
     </row>
     <row r="230">
@@ -5837,10 +5820,10 @@
         </is>
       </c>
       <c r="D231" t="n">
-        <v>0.001257</v>
+        <v>0.001</v>
       </c>
       <c r="E231" t="n">
-        <v>38186</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="232">
@@ -5875,10 +5858,10 @@
         </is>
       </c>
       <c r="D233" t="n">
-        <v>0.0015</v>
+        <v>0.001786</v>
       </c>
       <c r="E233" t="n">
-        <v>32000</v>
+        <v>26876</v>
       </c>
     </row>
     <row r="234">
@@ -5894,10 +5877,10 @@
         </is>
       </c>
       <c r="D234" t="n">
-        <v>0.001757</v>
+        <v>0.001471</v>
       </c>
       <c r="E234" t="n">
-        <v>27319</v>
+        <v>32631</v>
       </c>
     </row>
     <row r="235">
@@ -5970,10 +5953,10 @@
         </is>
       </c>
       <c r="D238" t="n">
-        <v>0.001257</v>
+        <v>0.001543</v>
       </c>
       <c r="E238" t="n">
-        <v>38186</v>
+        <v>31108</v>
       </c>
     </row>
     <row r="239">
@@ -6008,10 +5991,10 @@
         </is>
       </c>
       <c r="D240" t="n">
-        <v>0.001343</v>
+        <v>0.001629</v>
       </c>
       <c r="E240" t="n">
-        <v>35741</v>
+        <v>29466</v>
       </c>
     </row>
     <row r="241">
@@ -6065,10 +6048,10 @@
         </is>
       </c>
       <c r="D243" t="n">
-        <v>0.001914</v>
+        <v>0.001629</v>
       </c>
       <c r="E243" t="n">
-        <v>25078</v>
+        <v>29466</v>
       </c>
     </row>
     <row r="244">
@@ -6103,10 +6086,10 @@
         </is>
       </c>
       <c r="D245" t="n">
-        <v>0.001314</v>
+        <v>0.0016</v>
       </c>
       <c r="E245" t="n">
-        <v>36530</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="246">
@@ -6175,14 +6158,14 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE15')</t>
+          <t>('SBS4', 'UE13')</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>0.001471</v>
+        <v>0.0019</v>
       </c>
       <c r="E249" t="n">
-        <v>32631</v>
+        <v>25263</v>
       </c>
     </row>
     <row r="250">
@@ -6194,14 +6177,14 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE22')</t>
+          <t>('SBS4', 'UE15')</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>0.0013</v>
+        <v>0.001471</v>
       </c>
       <c r="E250" t="n">
-        <v>36923</v>
+        <v>32631</v>
       </c>
     </row>
     <row r="251">
@@ -6213,14 +6196,14 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE23')</t>
+          <t>('SBS4', 'UE19')</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>0.001229</v>
+        <v>0.001771</v>
       </c>
       <c r="E251" t="n">
-        <v>39056</v>
+        <v>27103</v>
       </c>
     </row>
     <row r="252">
@@ -6232,14 +6215,14 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE24')</t>
+          <t>('SBS4', 'UE22')</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>0.001614</v>
+        <v>0.001014</v>
       </c>
       <c r="E252" t="n">
-        <v>29740</v>
+        <v>47337</v>
       </c>
     </row>
     <row r="253">
@@ -6251,14 +6234,14 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE25')</t>
+          <t>('SBS4', 'UE23')</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>0.001171</v>
+        <v>0.001</v>
       </c>
       <c r="E253" t="n">
-        <v>40991</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="254">
@@ -6270,14 +6253,14 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE27')</t>
+          <t>('SBS4', 'UE24')</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>0.001757</v>
+        <v>0.001329</v>
       </c>
       <c r="E254" t="n">
-        <v>27319</v>
+        <v>36117</v>
       </c>
     </row>
     <row r="255">
@@ -6289,14 +6272,14 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE29')</t>
+          <t>('SBS4', 'UE25')</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>0.0016</v>
+        <v>0.001</v>
       </c>
       <c r="E255" t="n">
-        <v>30000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="256">
@@ -6308,14 +6291,14 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE32')</t>
+          <t>('SBS4', 'UE27')</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>0.001886</v>
+        <v>0.0019</v>
       </c>
       <c r="E256" t="n">
-        <v>25451</v>
+        <v>25263</v>
       </c>
     </row>
     <row r="257">
@@ -6327,14 +6310,14 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE34')</t>
+          <t>('SBS4', 'UE29')</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>0.001943</v>
+        <v>0.001886</v>
       </c>
       <c r="E257" t="n">
-        <v>24704</v>
+        <v>25451</v>
       </c>
     </row>
     <row r="258">
@@ -6346,14 +6329,14 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE35')</t>
+          <t>('SBS4', 'UE34')</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>0.001186</v>
+        <v>0.001943</v>
       </c>
       <c r="E258" t="n">
-        <v>40472</v>
+        <v>24704</v>
       </c>
     </row>
     <row r="259">
@@ -6365,14 +6348,14 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE37')</t>
+          <t>('SBS4', 'UE35')</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>0.001443</v>
+        <v>0.001</v>
       </c>
       <c r="E259" t="n">
-        <v>33264</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="260">
@@ -6384,14 +6367,14 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>('SBS4', 'UE43')</t>
+          <t>('SBS4', 'UE37')</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>0.0019</v>
+        <v>0.001729</v>
       </c>
       <c r="E260" t="n">
-        <v>25263</v>
+        <v>27762</v>
       </c>
     </row>
     <row r="261">
@@ -6411,6 +6394,25 @@
       </c>
       <c r="E261" t="n">
         <v>32301</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="n">
+        <v>2</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>('SBS4', 'UE48')</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>0.001986</v>
+      </c>
+      <c r="E262" t="n">
+        <v>24169</v>
       </c>
     </row>
   </sheetData>
@@ -6458,11 +6460,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['00000001_F9']</t>
+          <t>['00000001_F3']</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.0018</v>
+        <v>0.0013</v>
       </c>
     </row>
     <row r="3">
@@ -6474,11 +6476,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['00000002_F6']</t>
+          <t>['00000002_F9']</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.0011</v>
+        <v>0.0017</v>
       </c>
     </row>
     <row r="4">
@@ -6490,11 +6492,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['00000003_F2']</t>
+          <t>['00000003_F1']</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.0015</v>
+        <v>0.0011</v>
       </c>
     </row>
     <row r="5">
@@ -6506,11 +6508,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['00000001_F9']</t>
+          <t>['00000001_F3']</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.001943</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="6">
@@ -6522,11 +6524,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['00000002_F6']</t>
+          <t>['00000002_F9']</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.004</v>
+        <v>0.001871</v>
       </c>
     </row>
     <row r="7">
@@ -6538,11 +6540,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['00000003_F2']</t>
+          <t>['00000003_F1']</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="8">
@@ -6554,11 +6556,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['00000004_F2']</t>
+          <t>['00000004_F1']</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.004</v>
+        <v>0.001657</v>
       </c>
     </row>
     <row r="9">
@@ -6570,11 +6572,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['00000005_F2']</t>
+          <t>['00000005_F3']</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="10">
@@ -6586,11 +6588,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['00000006_F6']</t>
+          <t>['00000006_F5']</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.004</v>
+        <v>0.0014</v>
       </c>
     </row>
   </sheetData>
@@ -6834,10 +6836,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="F8" t="n">
         <v>8000</v>
@@ -6922,10 +6924,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="F12" t="n">
         <v>8000</v>
@@ -6944,10 +6946,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E13" t="n">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="F13" t="n">
         <v>8000</v>
@@ -6966,10 +6968,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="F14" t="n">
         <v>8000</v>
@@ -7079,16 +7081,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1667</v>
+        <v>0.6667</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8333</v>
+        <v>0.3333</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
         <v>6</v>
@@ -7191,13 +7193,13 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2" t="n">
         <v>4</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3">
@@ -7226,13 +7228,13 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J3" t="n">
         <v>4</v>
       </c>
       <c r="K3" t="n">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>
@@ -7379,10 +7381,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08695652173913043</v>
+        <v>0.08955223880597014</v>
       </c>
     </row>
   </sheetData>
@@ -7466,7 +7468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE17')</t>
+          <t>('SBS2', 'UE48')</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -7482,7 +7484,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE49')</t>
+          <t>('SBS3', 'UE43')</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -7498,7 +7500,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>('SBS3', 'UE31')</t>
+          <t>('SBS4', 'UE29')</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -7514,7 +7516,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>('MBS0', 'UE2')</t>
+          <t>('MBS0', 'UE25')</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -7530,7 +7532,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>('MBS0', 'UE24')</t>
+          <t>('MBS0', 'UE48')</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -7546,7 +7548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>('MBS0', 'UE31')</t>
+          <t>('SBS1', 'UE29')</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -7562,7 +7564,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>('MBS0', 'UE42')</t>
+          <t>('SBS2', 'UE2')</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -7578,7 +7580,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>('MBS0', 'UE49')</t>
+          <t>('SBS3', 'UE32')</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -7594,7 +7596,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>('SBS2', 'UE17')</t>
+          <t>('SBS3', 'UE43')</t>
         </is>
       </c>
       <c r="D10" t="n">

</xml_diff>